<commit_message>
update pdf and xslx files
</commit_message>
<xml_diff>
--- a/04-item-allocation/code/winner.xlsx
+++ b/04-item-allocation/code/winner.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="x" vbProcedure="false">Sheet1!$B$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="x" vbProcedure="false">Sheet2!$B$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="x" vbProcedure="false">Sheet2!$B$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <r>
       <rPr>
@@ -98,7 +98,7 @@
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ישראל ביתנו</t>
+      <t xml:space="preserve">דונאלד</t>
     </r>
     <r>
       <rPr>
@@ -118,7 +118,7 @@
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">כולנו</t>
+      <t xml:space="preserve">איואנה</t>
     </r>
     <r>
       <rPr>
@@ -211,7 +211,30 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">(65+30x)/10 = (30+40(1-x))/6</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(x = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nachlieli CLM"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">כמה איואנה מקבלת מהחפץ שחולק</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -291,46 +314,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">r:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Nachlieli CLM"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">דונאלד</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Nachlieli CLM"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">איואנה</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
     </r>
   </si>
 </sst>
@@ -338,9 +321,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -500,7 +484,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,7 +492,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,7 +520,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -544,7 +528,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,7 +613,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -832,79 +816,82 @@
         <f aca="false">_xlfn.CONCAT(F8,"+",G3,"x = ",H7,"+",G2,"(1-x)")</f>
         <v>65+30x = 30+40(1-x)</v>
       </c>
-      <c r="I10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B12" s="1" t="n">
         <f aca="false">(H7-F8+G2)/(G3+G2)</f>
         <v>0.0714285714285714</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="17" t="n">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="17" t="n">
         <f aca="false">H7+(1-x)*G2</f>
         <v>67.1428571428571</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="H14" s="14"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17" t="n">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="n">
         <f aca="false">F8+x*G3</f>
         <v>67.1428571428571</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="16" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
+      <c r="H15" s="17"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="17" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="n">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19" t="n">
         <f aca="false">C3*$G$5</f>
         <v>53.3333333333333</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19" t="n">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19" t="n">
         <f aca="false">E3*$G$5</f>
         <v>33.3333333333333</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19" t="n">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19" t="n">
         <f aca="false">G3*$G$5</f>
         <v>40</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19" t="n">
+      <c r="H17" s="19"/>
+      <c r="I17" s="19" t="n">
         <f aca="false">I3*$G$5</f>
         <v>6.66666666666667</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -970,7 +957,7 @@
     </row>
     <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="n">
@@ -996,7 +983,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="n">

</xml_diff>